<commit_message>
new 2k patch adjustments
</commit_message>
<xml_diff>
--- a/extractor.xlsx
+++ b/extractor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\2k21Extractor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9138B0C-353E-420B-8989-820FD451FFE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14BA5C64-A5EB-4625-A682-D0FA4EDE0C13}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5490" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5415" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="player stats" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H3:H21"/>
     </sheetView>
   </sheetViews>
@@ -1118,8 +1118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C274F46-7B49-4EDC-9C0A-0AA13FFBC626}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>